<commit_message>
added data validatin to switch worksheets column a
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -7965,7 +7965,10 @@
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:I2"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation sqref="A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 A30 A31 A32 A33 A34 A35 A36 A37 A38 A39 A40 A41 A42 A43 A44 A45 A46 A47 A48 A49 A50 A51 A52 A53 A54 A55 A56 A57 A58 A59 A60 A61 A62 A63 A64 A65 A66 A67 A68 A69 A70 A71 A72 A73 A74 A75 A76 A77 A78 A79 A80 A81 A82 A83 A84 A85 A86 A87 A88 A89 A90 A91 A92 A93 A94 A95 A96 A97 A98 A99 A100 A101 A102 A103 A104 A105 A106 A107 A108 A109 A110 A111 A112 A113 A114 A115 A116 A117 A118 A119 A120 A121 A122 A123 A124 A125 A126 A127 A128 A129 A130 A131 A132 A133 A134 A135 A136 A137 A138 A139 A140 A141 A142 A143 A144 A145 A146 A147 A148 A149 A150 A151 A152 A153 A154 A155 A156 A157 A158 A159 A160 A161 A162 A163 A164 A165 A166 A167 A168 A169 A170 A171 A172 A173 A174 A175 A176 A177 A178 A179 A180 A181 A182 A183 A184 A185 A186 A187 A188 A189 A190 A191 A192 A193 A194 A195 A196 A197 A198 A199 A200 A201 A202 A203" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"intf_selector"</formula1>
+    </dataValidation>
     <dataValidation sqref="E4 E5 E6 E7 E8 E9 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25 E26 E27 E28 E29 E30 E31 E32 E33 E34 E35 E36 E37 E38 E39 E40 E41 E42 E43 E44 E45 E46 E47 E48 E49 E50 E51 E52 E53 E54 E55 E56 E57 E58 E59 E60 E61 E62 E63 E64 E65 E66 E67 E68 E69 E70 E71 E72 E73 E74 E75 E76 E77 E78 E79 E80 E81 E82 E83 E84 E85 E86 E87 E88 E89 E90 E91 E92 E93 E94 E95 E96 E97 E98 E99 E100 E101 E102 E103 E104 E105 E106 E107 E108 E109 E110 E111 E112 E113 E114 E115 E116 E117 E118 E119 E120 E121 E122 E123 E124 E125 E126 E127 E128 E129 E130 E131 E132 E133 E134 E135 E136 E137 E138 E139 E140 E141 E142 E143 E144 E145 E146 E147 E148 E149 E150 E151 E152 E153 E154 E155 E156 E157 E158 E159 E160 E161 E162 E163 E164 E165 E166 E167 E168 E169 E170 E171 E172 E173 E174 E175 E176 E177 E178 E179 E180 E181 E182 E183 E184 E185 E186 E187 E188 E189 E190 E191 E192 E193 E194 E195 E196 E197 E198 E199 E200 E201 E202 E203" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"access,breakout,bundle"</formula1>
     </dataValidation>
@@ -9323,7 +9326,10 @@
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:I2"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation sqref="A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 A30 A31 A32 A33 A34 A35 A36 A37 A38 A39 A40 A41 A42 A43 A44 A45 A46 A47 A48 A49 A50 A51 A52 A53 A54 A55 A56 A57" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"intf_selector"</formula1>
+    </dataValidation>
     <dataValidation sqref="E4 E5 E6 E7 E8 E9 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25 E26 E27 E28 E29 E30 E31 E32 E33 E34 E35 E36 E37 E38 E39 E40 E41 E42 E43 E44 E45 E46 E47 E48 E49 E50 E51 E52 E53 E54 E55 E56 E57" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"access,breakout,bundle"</formula1>
     </dataValidation>
@@ -10681,7 +10687,10 @@
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:I2"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation sqref="A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 A30 A31 A32 A33 A34 A35 A36 A37 A38 A39 A40 A41 A42 A43 A44 A45 A46 A47 A48 A49 A50 A51 A52 A53 A54 A55 A56 A57" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"intf_selector"</formula1>
+    </dataValidation>
     <dataValidation sqref="E4 E5 E6 E7 E8 E9 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25 E26 E27 E28 E29 E30 E31 E32 E33 E34 E35 E36 E37 E38 E39 E40 E41 E42 E43 E44 E45 E46 E47 E48 E49 E50 E51 E52 E53 E54 E55 E56 E57" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"access,breakout,bundle"</formula1>
     </dataValidation>

</xml_diff>